<commit_message>
Updated the code for all test cases.
</commit_message>
<xml_diff>
--- a/src/test/java/testdata/Details.xlsx
+++ b/src/test/java/testdata/Details.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SHEGDE\SAHANA\CourseQA\HRManagement\src\test\java\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BEB6F113-1D57-4985-A57E-0143C170E8B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18E6703C-A9CA-400C-BC8B-379423CF9B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3260" yWindow="3110" windowWidth="14400" windowHeight="8170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>username     password</t>
   </si>
@@ -34,15 +34,6 @@
   </si>
   <si>
     <t>admin123</t>
-  </si>
-  <si>
-    <t>abcd</t>
-  </si>
-  <si>
-    <t>sahu</t>
-  </si>
-  <si>
-    <t>xyz</t>
   </si>
 </sst>
 </file>
@@ -66,7 +57,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -74,13 +65,29 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -363,11 +370,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -376,33 +381,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
+      <c r="B1" s="2"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>